<commit_message>
Add units and field type to google doc and implemented them in dgToScheme.R
</commit_message>
<xml_diff>
--- a/inst/googlesheet/emeScheme.xlsx
+++ b/inst/googlesheet/emeScheme.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="104">
   <si>
     <t>Property_Level_1</t>
   </si>
@@ -78,10 +78,10 @@
     <t>ExperimentalDesign</t>
   </si>
   <si>
-    <t>noTreatments</t>
-  </si>
-  <si>
-    <t>noReplicatesPerTreatment</t>
+    <t>noTreatments (count) [integer]</t>
+  </si>
+  <si>
+    <t>noReplicatesPerTreatment (count) [integer]</t>
   </si>
   <si>
     <t>description</t>
@@ -102,7 +102,7 @@
     <t>type</t>
   </si>
   <si>
-    <t>volume</t>
+    <t>volume (ml) [numeric]</t>
   </si>
   <si>
     <t>covers</t>
@@ -111,7 +111,7 @@
     <t>Shakers</t>
   </si>
   <si>
-    <t>speed (rpm)</t>
+    <t>speed (rpm) [integer]</t>
   </si>
   <si>
     <t>Species</t>
@@ -126,15 +126,12 @@
     <t>source</t>
   </si>
   <si>
-    <t>density (cells/ml)</t>
+    <t>density (cells/ml) [numeric]</t>
   </si>
   <si>
     <t>CultureMedium</t>
   </si>
   <si>
-    <t>volume (ml)</t>
-  </si>
-  <si>
     <t>BacteriaFlagellates</t>
   </si>
   <si>
@@ -156,31 +153,31 @@
     <t>InitialConditions</t>
   </si>
   <si>
-    <t>runInTime (hours)</t>
+    <t>runInTime (hours) [integer]</t>
   </si>
   <si>
     <t>Temperature</t>
   </si>
   <si>
-    <t>temperature (C)</t>
-  </si>
-  <si>
-    <t>temperature range</t>
-  </si>
-  <si>
-    <t>temperature change rate</t>
+    <t>temperature (C) [numeric]</t>
+  </si>
+  <si>
+    <t>temperatureRange (C)</t>
+  </si>
+  <si>
+    <t>temperatureChangeRate</t>
   </si>
   <si>
     <t>Light</t>
   </si>
   <si>
-    <t xml:space="preserve">intensity </t>
-  </si>
-  <si>
-    <t>frequency</t>
-  </si>
-  <si>
-    <t>photoperiod</t>
+    <t>intensity (lx) [numeric]</t>
+  </si>
+  <si>
+    <t>colour (nm) [integer]</t>
+  </si>
+  <si>
+    <t>photoperiod (h) [numeric]</t>
   </si>
   <si>
     <t>FinalConditions</t>
@@ -192,22 +189,25 @@
     <t>DuringExperimentMaintenance</t>
   </si>
   <si>
-    <t>initial density (cells/ml)</t>
-  </si>
-  <si>
-    <t>density changes</t>
-  </si>
-  <si>
-    <t>ecological role in treatment</t>
+    <t>initialDensity (cells/ml) [numeric]</t>
+  </si>
+  <si>
+    <t>densityChanges</t>
+  </si>
+  <si>
+    <t>ecologicalRoleInTreatment</t>
   </si>
   <si>
     <t>initial density</t>
   </si>
   <si>
+    <t>colour (nm) [numeric]</t>
+  </si>
+  <si>
     <t>Dispersal</t>
   </si>
   <si>
-    <t>spatial structure</t>
+    <t>spatialStructure</t>
   </si>
   <si>
     <t>change</t>
@@ -216,7 +216,7 @@
     <t>Nutrients</t>
   </si>
   <si>
-    <t>change in treatment</t>
+    <t>changeInTreatment</t>
   </si>
   <si>
     <t>Viscosity</t>
@@ -234,10 +234,10 @@
     <t>Sampling</t>
   </si>
   <si>
-    <t>frequency (days between samples)</t>
-  </si>
-  <si>
-    <t>replacement medium type</t>
+    <t>frequency (daysBetweenSamples) [numeric]</t>
+  </si>
+  <si>
+    <t>replacementMediumType</t>
   </si>
   <si>
     <t>Measuring</t>
@@ -249,13 +249,13 @@
     <t>preparation</t>
   </si>
   <si>
-    <t>type of microscope</t>
-  </si>
-  <si>
-    <t>microscopy method</t>
-  </si>
-  <si>
-    <t>comment (e.g. species)</t>
+    <t>typeOfMicroscope</t>
+  </si>
+  <si>
+    <t>microscopyMethod</t>
+  </si>
+  <si>
+    <t>comment (e.g.Species)</t>
   </si>
   <si>
     <t>VideoRecording</t>
@@ -273,22 +273,25 @@
     <t>resolution</t>
   </si>
   <si>
-    <t>length of recording (sec)</t>
-  </si>
-  <si>
-    <t>frame rate (per second)</t>
-  </si>
-  <si>
-    <t>colour space</t>
-  </si>
-  <si>
-    <t>light intensity</t>
-  </si>
-  <si>
-    <t>light colour</t>
-  </si>
-  <si>
-    <t>video format</t>
+    <t>colourSpace</t>
+  </si>
+  <si>
+    <t>lengthOfRecording (sec) [numeric]</t>
+  </si>
+  <si>
+    <t>frameRate (perSecond) [integer]</t>
+  </si>
+  <si>
+    <t>lightIntensity (lx) [numeric]</t>
+  </si>
+  <si>
+    <t>lightColour (nm) [numeric]</t>
+  </si>
+  <si>
+    <t>videoFormat</t>
+  </si>
+  <si>
+    <t>comment (e.g.species)</t>
   </si>
   <si>
     <t>FlowCam</t>
@@ -303,10 +306,10 @@
     <t>BacterialDensityFlowcytometry</t>
   </si>
   <si>
-    <t>type, version, …</t>
-  </si>
-  <si>
-    <t>settings parameter</t>
+    <t>typeVersion</t>
+  </si>
+  <si>
+    <t>settingsParameter</t>
   </si>
   <si>
     <t>DNABarcoding</t>
@@ -315,7 +318,7 @@
     <t>Respirometry</t>
   </si>
   <si>
-    <t>more details needed</t>
+    <t>moreDetailsNeeded</t>
   </si>
   <si>
     <t>NutrientsDecomposition</t>
@@ -333,10 +336,10 @@
     <t>VideoAnalysis</t>
   </si>
   <si>
-    <t>analysis method</t>
-  </si>
-  <si>
-    <t>parameter used</t>
+    <t>analysisMethod</t>
+  </si>
+  <si>
+    <t>parameterUsed</t>
   </si>
   <si>
     <t>FlowCamAnalysis</t>
@@ -709,6 +712,9 @@
     <xf borderId="10" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="4" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="10" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -717,9 +723,6 @@
     </xf>
     <xf borderId="10" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -766,8 +769,9 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="37.43"/>
     <col customWidth="1" min="2" max="2" width="36.57"/>
-    <col customWidth="1" min="3" max="3" width="27.14"/>
-    <col customWidth="1" min="4" max="5" width="24.14"/>
+    <col customWidth="1" min="3" max="3" width="41.71"/>
+    <col customWidth="1" min="4" max="4" width="25.43"/>
+    <col customWidth="1" min="5" max="5" width="24.14"/>
   </cols>
   <sheetData>
     <row r="1" ht="39.0" customHeight="1">
@@ -981,7 +985,7 @@
       <c r="B23" s="17"/>
       <c r="C23" s="18"/>
       <c r="D23" s="9" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E23" s="26"/>
     </row>
@@ -998,7 +1002,7 @@
       <c r="A25" s="15"/>
       <c r="B25" s="15"/>
       <c r="C25" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D25" s="24"/>
       <c r="E25" s="4"/>
@@ -1026,7 +1030,7 @@
       <c r="B28" s="17"/>
       <c r="C28" s="18"/>
       <c r="D28" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E28" s="26"/>
     </row>
@@ -1034,7 +1038,7 @@
       <c r="A29" s="15"/>
       <c r="B29" s="15"/>
       <c r="C29" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D29" s="24"/>
       <c r="E29" s="4"/>
@@ -1052,7 +1056,7 @@
       <c r="A31" s="15"/>
       <c r="B31" s="15"/>
       <c r="C31" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D31" s="24"/>
       <c r="E31" s="4"/>
@@ -1070,7 +1074,7 @@
       <c r="A33" s="15"/>
       <c r="B33" s="15"/>
       <c r="C33" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D33" s="24"/>
       <c r="E33" s="4"/>
@@ -1087,7 +1091,7 @@
     <row r="35" ht="24.75" customHeight="1">
       <c r="A35" s="3"/>
       <c r="B35" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C35" s="24"/>
       <c r="D35" s="24"/>
@@ -1097,7 +1101,7 @@
       <c r="A36" s="15"/>
       <c r="B36" s="15"/>
       <c r="C36" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D36" s="24"/>
       <c r="E36" s="4"/>
@@ -1114,17 +1118,17 @@
     <row r="38" ht="24.75" customHeight="1">
       <c r="A38" s="17"/>
       <c r="B38" s="17"/>
-      <c r="C38" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D38" s="18"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="E38" s="26"/>
     </row>
     <row r="39" ht="24.75" customHeight="1">
       <c r="A39" s="15"/>
       <c r="B39" s="15"/>
       <c r="C39" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D39" s="24"/>
       <c r="E39" s="4"/>
@@ -1134,7 +1138,7 @@
       <c r="B40" s="17"/>
       <c r="C40" s="27"/>
       <c r="D40" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E40" s="26"/>
     </row>
@@ -1142,8 +1146,8 @@
       <c r="A41" s="17"/>
       <c r="B41" s="17"/>
       <c r="C41" s="27"/>
-      <c r="D41" s="25" t="s">
-        <v>36</v>
+      <c r="D41" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="E41" s="26"/>
     </row>
@@ -1152,7 +1156,7 @@
       <c r="B42" s="17"/>
       <c r="C42" s="27"/>
       <c r="D42" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E42" s="26"/>
     </row>
@@ -1160,7 +1164,7 @@
       <c r="A43" s="15"/>
       <c r="B43" s="15"/>
       <c r="C43" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D43" s="24"/>
       <c r="E43" s="4"/>
@@ -1169,8 +1173,8 @@
       <c r="A44" s="17"/>
       <c r="B44" s="17"/>
       <c r="C44" s="27"/>
-      <c r="D44" s="25" t="s">
-        <v>39</v>
+      <c r="D44" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="E44" s="26"/>
     </row>
@@ -1178,8 +1182,8 @@
       <c r="A45" s="17"/>
       <c r="B45" s="17"/>
       <c r="C45" s="27"/>
-      <c r="D45" s="25" t="s">
-        <v>40</v>
+      <c r="D45" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="E45" s="26"/>
     </row>
@@ -1187,8 +1191,8 @@
       <c r="A46" s="17"/>
       <c r="B46" s="17"/>
       <c r="C46" s="27"/>
-      <c r="D46" s="25" t="s">
-        <v>41</v>
+      <c r="D46" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="E46" s="26"/>
     </row>
@@ -1196,7 +1200,7 @@
       <c r="A47" s="15"/>
       <c r="B47" s="15"/>
       <c r="C47" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D47" s="24"/>
       <c r="E47" s="4"/>
@@ -1212,7 +1216,7 @@
     </row>
     <row r="49" ht="24.75" customHeight="1">
       <c r="A49" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B49" s="24"/>
       <c r="C49" s="24"/>
@@ -1222,7 +1226,7 @@
     <row r="50" ht="24.75" customHeight="1">
       <c r="A50" s="15"/>
       <c r="B50" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C50" s="24"/>
       <c r="D50" s="4"/>
@@ -1258,8 +1262,8 @@
     <row r="54" ht="24.75" customHeight="1">
       <c r="A54" s="18"/>
       <c r="B54" s="18"/>
-      <c r="C54" s="26" t="s">
-        <v>45</v>
+      <c r="C54" s="29" t="s">
+        <v>44</v>
       </c>
       <c r="D54" s="26"/>
       <c r="E54" s="26"/>
@@ -1267,8 +1271,8 @@
     <row r="55" ht="24.75" customHeight="1">
       <c r="A55" s="18"/>
       <c r="B55" s="18"/>
-      <c r="C55" s="26" t="s">
-        <v>46</v>
+      <c r="C55" s="29" t="s">
+        <v>45</v>
       </c>
       <c r="D55" s="26"/>
       <c r="E55" s="26"/>
@@ -1276,8 +1280,8 @@
     <row r="56" ht="24.75" customHeight="1">
       <c r="A56" s="18"/>
       <c r="B56" s="18"/>
-      <c r="C56" s="29" t="s">
-        <v>47</v>
+      <c r="C56" s="30" t="s">
+        <v>46</v>
       </c>
       <c r="D56" s="28"/>
       <c r="E56" s="28"/>
@@ -1285,7 +1289,7 @@
     <row r="57" ht="24.75" customHeight="1">
       <c r="A57" s="15"/>
       <c r="B57" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C57" s="24"/>
       <c r="D57" s="24"/>
@@ -1304,7 +1308,7 @@
       <c r="A59" s="17"/>
       <c r="B59" s="18"/>
       <c r="C59" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
@@ -1313,7 +1317,7 @@
       <c r="A60" s="17"/>
       <c r="B60" s="18"/>
       <c r="C60" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
@@ -1321,7 +1325,7 @@
     <row r="61" ht="24.75" customHeight="1">
       <c r="A61" s="24"/>
       <c r="B61" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C61" s="24"/>
       <c r="D61" s="4"/>
@@ -1331,7 +1335,7 @@
       <c r="A62" s="18"/>
       <c r="B62" s="18"/>
       <c r="C62" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D62" s="26"/>
       <c r="E62" s="26"/>
@@ -1339,8 +1343,8 @@
     <row r="63" ht="24.75" customHeight="1">
       <c r="A63" s="18"/>
       <c r="B63" s="18"/>
-      <c r="C63" s="25" t="s">
-        <v>36</v>
+      <c r="C63" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="D63" s="26"/>
       <c r="E63" s="26"/>
@@ -1349,7 +1353,7 @@
       <c r="A64" s="18"/>
       <c r="B64" s="18"/>
       <c r="C64" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D64" s="26"/>
       <c r="E64" s="26"/>
@@ -1357,7 +1361,7 @@
     <row r="65" ht="24.75" customHeight="1">
       <c r="A65" s="24"/>
       <c r="B65" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C65" s="24"/>
       <c r="D65" s="4"/>
@@ -1366,8 +1370,8 @@
     <row r="66" ht="24.75" customHeight="1">
       <c r="A66" s="18"/>
       <c r="B66" s="18"/>
-      <c r="C66" s="25" t="s">
-        <v>39</v>
+      <c r="C66" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="D66" s="26"/>
       <c r="E66" s="26"/>
@@ -1375,8 +1379,8 @@
     <row r="67" ht="24.75" customHeight="1">
       <c r="A67" s="18"/>
       <c r="B67" s="18"/>
-      <c r="C67" s="25" t="s">
-        <v>40</v>
+      <c r="C67" s="9" t="s">
+        <v>48</v>
       </c>
       <c r="D67" s="26"/>
       <c r="E67" s="26"/>
@@ -1384,8 +1388,8 @@
     <row r="68" ht="24.75" customHeight="1">
       <c r="A68" s="18"/>
       <c r="B68" s="18"/>
-      <c r="C68" s="25" t="s">
-        <v>41</v>
+      <c r="C68" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="D68" s="26"/>
       <c r="E68" s="26"/>
@@ -1422,14 +1426,14 @@
       <c r="B72" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C72" s="30"/>
+      <c r="C72" s="31"/>
       <c r="D72" s="4"/>
       <c r="E72" s="4"/>
     </row>
     <row r="73" ht="24.75" customHeight="1">
       <c r="A73" s="18"/>
       <c r="B73" s="18"/>
-      <c r="C73" s="25" t="s">
+      <c r="C73" s="9" t="s">
         <v>53</v>
       </c>
       <c r="D73" s="26"/>
@@ -1440,14 +1444,14 @@
       <c r="B74" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C74" s="31"/>
+      <c r="C74" s="32"/>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
     </row>
     <row r="75" ht="24.75" customHeight="1">
       <c r="A75" s="27"/>
       <c r="B75" s="23"/>
-      <c r="C75" s="32" t="s">
+      <c r="C75" s="29" t="s">
         <v>9</v>
       </c>
       <c r="D75" s="26"/>
@@ -1465,7 +1469,7 @@
     <row r="77" ht="24.75" customHeight="1">
       <c r="A77" s="27"/>
       <c r="B77" s="23"/>
-      <c r="C77" s="32" t="s">
+      <c r="C77" s="29" t="s">
         <v>14</v>
       </c>
       <c r="D77" s="26"/>
@@ -1474,7 +1478,7 @@
     <row r="78" ht="24.75" customHeight="1">
       <c r="A78" s="27"/>
       <c r="B78" s="23"/>
-      <c r="C78" s="29" t="s">
+      <c r="C78" s="30" t="s">
         <v>56</v>
       </c>
       <c r="D78" s="26"/>
@@ -1483,7 +1487,7 @@
     <row r="79" ht="24.75" customHeight="1">
       <c r="A79" s="27"/>
       <c r="B79" s="23"/>
-      <c r="C79" s="29" t="s">
+      <c r="C79" s="30" t="s">
         <v>51</v>
       </c>
       <c r="D79" s="26"/>
@@ -1501,7 +1505,7 @@
     <row r="81" ht="24.75" customHeight="1">
       <c r="A81" s="27"/>
       <c r="B81" s="23"/>
-      <c r="C81" s="32" t="s">
+      <c r="C81" s="29" t="s">
         <v>9</v>
       </c>
       <c r="D81" s="26"/>
@@ -1528,7 +1532,7 @@
     <row r="84" ht="24.75" customHeight="1">
       <c r="A84" s="17"/>
       <c r="B84" s="9" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C84" s="18"/>
       <c r="D84" s="26"/>
@@ -1565,7 +1569,7 @@
       <c r="A88" s="17"/>
       <c r="B88" s="18"/>
       <c r="C88" s="19" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D88" s="19"/>
       <c r="E88" s="19"/>
@@ -1582,7 +1586,7 @@
     <row r="90" ht="24.75" customHeight="1">
       <c r="A90" s="17"/>
       <c r="B90" s="18"/>
-      <c r="C90" s="25" t="s">
+      <c r="C90" s="9" t="s">
         <v>64</v>
       </c>
       <c r="D90" s="26"/>
@@ -1600,7 +1604,7 @@
     <row r="92" ht="24.75" customHeight="1">
       <c r="A92" s="17"/>
       <c r="B92" s="18"/>
-      <c r="C92" s="29" t="s">
+      <c r="C92" s="30" t="s">
         <v>66</v>
       </c>
       <c r="D92" s="26"/>
@@ -1619,7 +1623,7 @@
       <c r="A94" s="17"/>
       <c r="B94" s="18"/>
       <c r="C94" s="23" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D94" s="18"/>
       <c r="E94" s="18"/>
@@ -1681,7 +1685,7 @@
     <row r="101" ht="24.75" customHeight="1">
       <c r="A101" s="17"/>
       <c r="B101" s="18"/>
-      <c r="C101" s="23" t="s">
+      <c r="C101" s="30" t="s">
         <v>72</v>
       </c>
       <c r="D101" s="18"/>
@@ -1690,7 +1694,7 @@
     <row r="102" ht="24.75" customHeight="1">
       <c r="A102" s="17"/>
       <c r="B102" s="18"/>
-      <c r="C102" s="29" t="s">
+      <c r="C102" s="23" t="s">
         <v>73</v>
       </c>
       <c r="D102" s="18"/>
@@ -1699,16 +1703,16 @@
     <row r="103" ht="24.75" customHeight="1">
       <c r="A103" s="17"/>
       <c r="B103" s="18"/>
-      <c r="C103" s="29" t="s">
+      <c r="C103" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="D103" s="18"/>
+      <c r="D103" s="30"/>
       <c r="E103" s="18"/>
     </row>
     <row r="104" ht="24.75" customHeight="1">
       <c r="A104" s="17"/>
       <c r="B104" s="18"/>
-      <c r="C104" s="29" t="s">
+      <c r="C104" s="30" t="s">
         <v>75</v>
       </c>
       <c r="D104" s="18"/>
@@ -1717,7 +1721,7 @@
     <row r="105" ht="24.75" customHeight="1">
       <c r="A105" s="17"/>
       <c r="B105" s="18"/>
-      <c r="C105" s="29" t="s">
+      <c r="C105" s="30" t="s">
         <v>76</v>
       </c>
       <c r="D105" s="18"/>
@@ -1726,7 +1730,7 @@
     <row r="106" ht="24.75" customHeight="1">
       <c r="A106" s="17"/>
       <c r="B106" s="18"/>
-      <c r="C106" s="29" t="s">
+      <c r="C106" s="30" t="s">
         <v>77</v>
       </c>
       <c r="D106" s="18"/>
@@ -1735,8 +1739,8 @@
     <row r="107" ht="24.75" customHeight="1">
       <c r="A107" s="17"/>
       <c r="B107" s="18"/>
-      <c r="C107" s="29" t="s">
-        <v>66</v>
+      <c r="C107" s="30" t="s">
+        <v>78</v>
       </c>
       <c r="D107" s="18"/>
       <c r="E107" s="18"/>
@@ -1744,7 +1748,7 @@
     <row r="108" ht="24.75" customHeight="1">
       <c r="A108" s="15"/>
       <c r="B108" s="34" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C108" s="4"/>
       <c r="D108" s="24"/>
@@ -1763,7 +1767,7 @@
       <c r="A110" s="17"/>
       <c r="B110" s="18"/>
       <c r="C110" s="19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D110" s="18"/>
       <c r="E110" s="18"/>
@@ -1772,7 +1776,7 @@
       <c r="A111" s="17"/>
       <c r="B111" s="18"/>
       <c r="C111" s="19" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D111" s="18"/>
       <c r="E111" s="18"/>
@@ -1781,7 +1785,7 @@
       <c r="A112" s="17"/>
       <c r="B112" s="18"/>
       <c r="C112" s="20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D112" s="18"/>
       <c r="E112" s="18"/>
@@ -1789,7 +1793,7 @@
     <row r="113" ht="24.75" customHeight="1">
       <c r="A113" s="15"/>
       <c r="B113" s="16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C113" s="24"/>
       <c r="D113" s="4"/>
@@ -1798,8 +1802,8 @@
     <row r="114" ht="24.75" customHeight="1">
       <c r="A114" s="17"/>
       <c r="B114" s="35"/>
-      <c r="C114" s="25" t="s">
-        <v>82</v>
+      <c r="C114" s="9" t="s">
+        <v>83</v>
       </c>
       <c r="D114" s="26"/>
       <c r="E114" s="26"/>
@@ -1808,7 +1812,7 @@
       <c r="A115" s="17"/>
       <c r="B115" s="35"/>
       <c r="C115" s="19" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D115" s="26"/>
       <c r="E115" s="26"/>
@@ -1817,7 +1821,7 @@
       <c r="A116" s="17"/>
       <c r="B116" s="35"/>
       <c r="C116" s="36" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D116" s="26"/>
       <c r="E116" s="26"/>
@@ -1826,7 +1830,7 @@
       <c r="A117" s="17"/>
       <c r="B117" s="35"/>
       <c r="C117" s="25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D117" s="26"/>
       <c r="E117" s="26"/>
@@ -1834,7 +1838,7 @@
     <row r="118" ht="24.75" customHeight="1">
       <c r="A118" s="15"/>
       <c r="B118" s="16" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C118" s="24"/>
       <c r="D118" s="4"/>
@@ -1852,7 +1856,7 @@
     <row r="120" ht="24.75" customHeight="1">
       <c r="A120" s="15"/>
       <c r="B120" s="34" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C120" s="24"/>
       <c r="D120" s="4"/>
@@ -1871,7 +1875,7 @@
       <c r="A122" s="17"/>
       <c r="B122" s="38"/>
       <c r="C122" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D122" s="26"/>
       <c r="E122" s="26"/>
@@ -1879,7 +1883,7 @@
     <row r="123" ht="24.75" customHeight="1">
       <c r="A123" s="15"/>
       <c r="B123" s="16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C123" s="24"/>
       <c r="D123" s="4"/>
@@ -1889,14 +1893,14 @@
       <c r="A124" s="17"/>
       <c r="B124" s="38"/>
       <c r="C124" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D124" s="26"/>
       <c r="E124" s="26"/>
     </row>
     <row r="125" ht="24.75" customHeight="1">
       <c r="A125" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B125" s="24"/>
       <c r="C125" s="24"/>
@@ -1906,7 +1910,7 @@
     <row r="126" ht="24.75" customHeight="1">
       <c r="A126" s="15"/>
       <c r="B126" s="16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C126" s="24"/>
       <c r="D126" s="4"/>
@@ -1924,7 +1928,7 @@
     <row r="128" ht="24.75" customHeight="1">
       <c r="A128" s="15"/>
       <c r="B128" s="16" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C128" s="24"/>
       <c r="D128" s="4"/>
@@ -1934,7 +1938,7 @@
       <c r="A129" s="17"/>
       <c r="B129" s="18"/>
       <c r="C129" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D129" s="9"/>
       <c r="E129" s="9"/>
@@ -1943,7 +1947,7 @@
       <c r="A130" s="17"/>
       <c r="B130" s="18"/>
       <c r="C130" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D130" s="9"/>
       <c r="E130" s="9"/>
@@ -1951,7 +1955,7 @@
     <row r="131" ht="24.75" customHeight="1">
       <c r="A131" s="15"/>
       <c r="B131" s="16" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C131" s="4"/>
       <c r="D131" s="4"/>
@@ -1960,16 +1964,16 @@
     <row r="132" ht="24.75" customHeight="1">
       <c r="A132" s="17"/>
       <c r="B132" s="25"/>
-      <c r="C132" s="32" t="s">
+      <c r="C132" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D132" s="32"/>
-      <c r="E132" s="32"/>
+      <c r="D132" s="29"/>
+      <c r="E132" s="29"/>
     </row>
     <row r="133" ht="24.75" customHeight="1">
       <c r="A133" s="15"/>
       <c r="B133" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C133" s="24"/>
       <c r="D133" s="4"/>
@@ -1987,7 +1991,7 @@
     <row r="135" ht="24.75" customHeight="1">
       <c r="A135" s="15"/>
       <c r="B135" s="16" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C135" s="24"/>
       <c r="D135" s="4"/>
@@ -2005,7 +2009,7 @@
     <row r="137" ht="24.75" customHeight="1">
       <c r="A137" s="15"/>
       <c r="B137" s="16" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C137" s="24"/>
       <c r="D137" s="4"/>
@@ -2023,7 +2027,7 @@
     <row r="139" ht="24.75" customHeight="1">
       <c r="A139" s="15"/>
       <c r="B139" s="16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C139" s="24"/>
       <c r="D139" s="4"/>
@@ -2041,7 +2045,7 @@
     <row r="141" ht="24.75" customHeight="1">
       <c r="A141" s="15"/>
       <c r="B141" s="16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C141" s="24"/>
       <c r="D141" s="4"/>
@@ -2059,7 +2063,7 @@
     <row r="143" ht="24.75" customHeight="1">
       <c r="A143" s="15"/>
       <c r="B143" s="16" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C143" s="24"/>
       <c r="D143" s="4"/>
@@ -2077,7 +2081,7 @@
     <row r="145" ht="24.75" customHeight="1">
       <c r="A145" s="15"/>
       <c r="B145" s="16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C145" s="24"/>
       <c r="D145" s="4"/>
@@ -2095,7 +2099,7 @@
     <row r="147" ht="24.75" customHeight="1">
       <c r="A147" s="15"/>
       <c r="B147" s="16" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C147" s="24"/>
       <c r="D147" s="4"/>

</xml_diff>

<commit_message>
Updata Data using new definitions
</commit_message>
<xml_diff>
--- a/inst/googlesheet/emeScheme.xlsx
+++ b/inst/googlesheet/emeScheme.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="140">
   <si>
     <t>Property_Level_1</t>
   </si>
@@ -245,6 +245,9 @@
     <t>na</t>
   </si>
   <si>
+    <t>SpeciesTreatment</t>
+  </si>
+  <si>
     <t>initialDensity (cells/ml) [numeric]</t>
   </si>
   <si>
@@ -437,13 +440,13 @@
     <t>analysisMethod</t>
   </si>
   <si>
-    <t>bemovi</t>
+    <t>bemovi, bemovi 2</t>
   </si>
   <si>
     <t>parameterUsed</t>
   </si>
   <si>
-    <t>a = 1, b = 2, c = 3, x = 35</t>
+    <t>a = 1; b = 2; c = 3; x = 35, a = 10; b = 3; y = 9999</t>
   </si>
   <si>
     <t>FlowCamAnalysis</t>
@@ -1655,7 +1658,7 @@
     <row r="58" ht="24.75" customHeight="1">
       <c r="A58" s="29"/>
       <c r="B58" s="19" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
@@ -1678,19 +1681,19 @@
       <c r="A60" s="21"/>
       <c r="B60" s="21"/>
       <c r="C60" s="34" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D60" s="31"/>
       <c r="E60" s="31"/>
       <c r="F60" s="51" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="61" ht="24.75" customHeight="1">
       <c r="A61" s="21"/>
       <c r="B61" s="21"/>
       <c r="C61" s="34" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D61" s="31"/>
       <c r="E61" s="31"/>
@@ -1702,7 +1705,7 @@
       <c r="A62" s="21"/>
       <c r="B62" s="21"/>
       <c r="C62" s="35" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D62" s="33"/>
       <c r="E62" s="33"/>
@@ -1736,19 +1739,19 @@
       <c r="A65" s="20"/>
       <c r="B65" s="21"/>
       <c r="C65" s="11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D65" s="11"/>
       <c r="E65" s="11"/>
       <c r="F65" s="51" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="66" ht="24.75" customHeight="1">
       <c r="A66" s="20"/>
       <c r="B66" s="21"/>
       <c r="C66" s="11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D66" s="11"/>
       <c r="E66" s="11"/>
@@ -1788,7 +1791,7 @@
       <c r="D69" s="31"/>
       <c r="E69" s="31"/>
       <c r="F69" s="51" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" ht="24.75" customHeight="1">
@@ -1800,7 +1803,7 @@
       <c r="D70" s="31"/>
       <c r="E70" s="31"/>
       <c r="F70" s="51" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="71" ht="24.75" customHeight="1">
@@ -1829,7 +1832,7 @@
       <c r="A73" s="21"/>
       <c r="B73" s="21"/>
       <c r="C73" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D73" s="31"/>
       <c r="E73" s="31"/>
@@ -1852,7 +1855,7 @@
     <row r="75" ht="24.75" customHeight="1">
       <c r="A75" s="29"/>
       <c r="B75" s="19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C75" s="29"/>
       <c r="D75" s="5"/>
@@ -1863,7 +1866,7 @@
       <c r="A76" s="21"/>
       <c r="B76" s="21"/>
       <c r="C76" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D76" s="31"/>
       <c r="E76" s="31"/>
@@ -1873,7 +1876,7 @@
       <c r="A77" s="21"/>
       <c r="B77" s="21"/>
       <c r="C77" s="30" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D77" s="31"/>
       <c r="E77" s="31"/>
@@ -1882,7 +1885,7 @@
     <row r="78" ht="24.75" customHeight="1">
       <c r="A78" s="29"/>
       <c r="B78" s="19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C78" s="37"/>
       <c r="D78" s="5"/>
@@ -1893,7 +1896,7 @@
       <c r="A79" s="21"/>
       <c r="B79" s="21"/>
       <c r="C79" s="11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D79" s="31"/>
       <c r="E79" s="31"/>
@@ -1912,7 +1915,7 @@
     <row r="81" ht="24.75" customHeight="1">
       <c r="A81" s="29"/>
       <c r="B81" s="19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C81" s="38"/>
       <c r="D81" s="5"/>
@@ -1942,7 +1945,7 @@
     <row r="84" ht="24.75" customHeight="1">
       <c r="A84" s="39"/>
       <c r="B84" s="19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
@@ -1963,7 +1966,7 @@
       <c r="A86" s="32"/>
       <c r="B86" s="28"/>
       <c r="C86" s="35" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D86" s="31"/>
       <c r="E86" s="31"/>
@@ -1973,7 +1976,7 @@
       <c r="A87" s="32"/>
       <c r="B87" s="28"/>
       <c r="C87" s="35" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D87" s="31"/>
       <c r="E87" s="31"/>
@@ -1982,7 +1985,7 @@
     <row r="88" ht="24.75" customHeight="1">
       <c r="A88" s="29"/>
       <c r="B88" s="40" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C88" s="29"/>
       <c r="D88" s="5"/>
@@ -2011,7 +2014,7 @@
     </row>
     <row r="91" ht="24.75" customHeight="1">
       <c r="A91" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B91" s="29"/>
       <c r="C91" s="29"/>
@@ -2022,7 +2025,7 @@
     <row r="92" ht="24.75" customHeight="1">
       <c r="A92" s="20"/>
       <c r="B92" s="11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C92" s="21"/>
       <c r="D92" s="31"/>
@@ -2046,18 +2049,18 @@
     <row r="94" ht="24.75" customHeight="1">
       <c r="A94" s="20"/>
       <c r="B94" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C94" s="21"/>
       <c r="D94" s="31"/>
       <c r="E94" s="31"/>
       <c r="F94" s="51" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="95" ht="24.75" customHeight="1">
       <c r="A95" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B95" s="29"/>
       <c r="C95" s="29"/>
@@ -2068,7 +2071,7 @@
     <row r="96" ht="24.75" customHeight="1">
       <c r="A96" s="18"/>
       <c r="B96" s="19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C96" s="29"/>
       <c r="D96" s="5"/>
@@ -2084,61 +2087,61 @@
       <c r="D97" s="22"/>
       <c r="E97" s="22"/>
       <c r="F97" s="51" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="98" ht="24.75" customHeight="1">
       <c r="A98" s="20"/>
       <c r="B98" s="21"/>
       <c r="C98" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D98" s="31"/>
       <c r="E98" s="31"/>
       <c r="F98" s="51" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="99" ht="24.75" customHeight="1">
       <c r="A99" s="20"/>
       <c r="B99" s="21"/>
       <c r="C99" s="11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D99" s="31"/>
       <c r="E99" s="31"/>
       <c r="F99" s="51" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="100" ht="24.75" customHeight="1">
       <c r="A100" s="20"/>
       <c r="B100" s="21"/>
       <c r="C100" s="11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D100" s="31"/>
       <c r="E100" s="31"/>
       <c r="F100" s="51" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="101" ht="24.75" customHeight="1">
       <c r="A101" s="20"/>
       <c r="B101" s="21"/>
       <c r="C101" s="35" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D101" s="31"/>
       <c r="E101" s="31"/>
       <c r="F101" s="51" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="102" ht="24.75" customHeight="1">
       <c r="A102" s="18"/>
       <c r="B102" s="19" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C102" s="29"/>
       <c r="D102" s="5"/>
@@ -2161,7 +2164,7 @@
       <c r="A104" s="20"/>
       <c r="B104" s="21"/>
       <c r="C104" s="21" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D104" s="21"/>
       <c r="E104" s="21"/>
@@ -2171,19 +2174,19 @@
       <c r="A105" s="20"/>
       <c r="B105" s="21"/>
       <c r="C105" s="28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D105" s="21"/>
       <c r="E105" s="21"/>
       <c r="F105" s="51" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="106" ht="24.75" customHeight="1">
       <c r="A106" s="20"/>
       <c r="B106" s="21"/>
       <c r="C106" s="28" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D106" s="21"/>
       <c r="E106" s="21"/>
@@ -2195,19 +2198,19 @@
       <c r="A107" s="20"/>
       <c r="B107" s="21"/>
       <c r="C107" s="28" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D107" s="21"/>
       <c r="E107" s="21"/>
       <c r="F107" s="51" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="108" ht="24.75" customHeight="1">
       <c r="A108" s="20"/>
       <c r="B108" s="21"/>
       <c r="C108" s="28" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D108" s="21"/>
       <c r="E108" s="21"/>
@@ -2217,7 +2220,7 @@
       <c r="A109" s="20"/>
       <c r="B109" s="21"/>
       <c r="C109" s="28" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D109" s="21"/>
       <c r="E109" s="21"/>
@@ -2229,19 +2232,19 @@
       <c r="A110" s="20"/>
       <c r="B110" s="21"/>
       <c r="C110" s="35" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D110" s="21"/>
       <c r="E110" s="21"/>
       <c r="F110" s="51" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="111" ht="24.75" customHeight="1">
       <c r="A111" s="20"/>
       <c r="B111" s="21"/>
       <c r="C111" s="28" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D111" s="21"/>
       <c r="E111" s="21"/>
@@ -2253,7 +2256,7 @@
       <c r="A112" s="20"/>
       <c r="B112" s="21"/>
       <c r="C112" s="35" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D112" s="35"/>
       <c r="E112" s="21"/>
@@ -2265,7 +2268,7 @@
       <c r="A113" s="20"/>
       <c r="B113" s="21"/>
       <c r="C113" s="35" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D113" s="21"/>
       <c r="E113" s="21"/>
@@ -2277,7 +2280,7 @@
       <c r="A114" s="20"/>
       <c r="B114" s="21"/>
       <c r="C114" s="35" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D114" s="21"/>
       <c r="E114" s="21"/>
@@ -2287,19 +2290,19 @@
       <c r="A115" s="20"/>
       <c r="B115" s="21"/>
       <c r="C115" s="35" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D115" s="21"/>
       <c r="E115" s="21"/>
       <c r="F115" s="51" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="116" ht="24.75" customHeight="1">
       <c r="A116" s="20"/>
       <c r="B116" s="21"/>
       <c r="C116" s="35" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D116" s="21"/>
       <c r="E116" s="21"/>
@@ -2308,7 +2311,7 @@
     <row r="117" ht="24.75" customHeight="1">
       <c r="A117" s="18"/>
       <c r="B117" s="40" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C117" s="5"/>
       <c r="D117" s="29"/>
@@ -2329,7 +2332,7 @@
       <c r="A119" s="20"/>
       <c r="B119" s="21"/>
       <c r="C119" s="22" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D119" s="21"/>
       <c r="E119" s="21"/>
@@ -2349,7 +2352,7 @@
       <c r="A121" s="20"/>
       <c r="B121" s="21"/>
       <c r="C121" s="23" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D121" s="21"/>
       <c r="E121" s="21"/>
@@ -2358,7 +2361,7 @@
     <row r="122" ht="24.75" customHeight="1">
       <c r="A122" s="18"/>
       <c r="B122" s="19" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C122" s="29"/>
       <c r="D122" s="5"/>
@@ -2369,7 +2372,7 @@
       <c r="A123" s="20"/>
       <c r="B123" s="41"/>
       <c r="C123" s="11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D123" s="31"/>
       <c r="E123" s="31"/>
@@ -2389,7 +2392,7 @@
       <c r="A125" s="20"/>
       <c r="B125" s="41"/>
       <c r="C125" s="42" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D125" s="31"/>
       <c r="E125" s="31"/>
@@ -2399,7 +2402,7 @@
       <c r="A126" s="20"/>
       <c r="B126" s="41"/>
       <c r="C126" s="30" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D126" s="31"/>
       <c r="E126" s="31"/>
@@ -2408,7 +2411,7 @@
     <row r="127" ht="24.75" customHeight="1">
       <c r="A127" s="18"/>
       <c r="B127" s="19" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C127" s="29"/>
       <c r="D127" s="5"/>
@@ -2438,7 +2441,7 @@
     <row r="130" ht="24.75" customHeight="1">
       <c r="A130" s="18"/>
       <c r="B130" s="40" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C130" s="29"/>
       <c r="D130" s="5"/>
@@ -2459,7 +2462,7 @@
       <c r="A132" s="20"/>
       <c r="B132" s="44"/>
       <c r="C132" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D132" s="31"/>
       <c r="E132" s="31"/>
@@ -2468,7 +2471,7 @@
     <row r="133" ht="24.75" customHeight="1">
       <c r="A133" s="18"/>
       <c r="B133" s="19" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C133" s="29"/>
       <c r="D133" s="5"/>
@@ -2479,7 +2482,7 @@
       <c r="A134" s="20"/>
       <c r="B134" s="44"/>
       <c r="C134" s="11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D134" s="31"/>
       <c r="E134" s="31"/>
@@ -2497,7 +2500,7 @@
     </row>
     <row r="136" ht="24.75" customHeight="1">
       <c r="A136" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B136" s="29"/>
       <c r="C136" s="29"/>
@@ -2508,7 +2511,7 @@
     <row r="137" ht="24.75" customHeight="1">
       <c r="A137" s="18"/>
       <c r="B137" s="19" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C137" s="29"/>
       <c r="D137" s="5"/>
@@ -2524,7 +2527,7 @@
       <c r="D138" s="31"/>
       <c r="E138" s="31"/>
       <c r="F138" s="51" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="139" ht="24.75" customHeight="1">
@@ -2540,7 +2543,7 @@
     <row r="140" ht="24.75" customHeight="1">
       <c r="A140" s="18"/>
       <c r="B140" s="19" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C140" s="29"/>
       <c r="D140" s="5"/>
@@ -2551,30 +2554,30 @@
       <c r="A141" s="20"/>
       <c r="B141" s="21"/>
       <c r="C141" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D141" s="11"/>
       <c r="E141" s="11"/>
       <c r="F141" s="51" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="142" ht="24.75" customHeight="1">
       <c r="A142" s="20"/>
       <c r="B142" s="21"/>
       <c r="C142" s="11" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D142" s="11"/>
       <c r="E142" s="11"/>
       <c r="F142" s="51" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="143" ht="24.75" customHeight="1">
       <c r="A143" s="18"/>
       <c r="B143" s="19" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C143" s="5"/>
       <c r="D143" s="5"/>
@@ -2604,7 +2607,7 @@
     <row r="146" ht="24.75" customHeight="1">
       <c r="A146" s="18"/>
       <c r="B146" s="19" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C146" s="29"/>
       <c r="D146" s="5"/>
@@ -2634,7 +2637,7 @@
     <row r="149" ht="24.75" customHeight="1">
       <c r="A149" s="18"/>
       <c r="B149" s="19" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C149" s="29"/>
       <c r="D149" s="5"/>
@@ -2664,7 +2667,7 @@
     <row r="152" ht="24.75" customHeight="1">
       <c r="A152" s="18"/>
       <c r="B152" s="19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C152" s="29"/>
       <c r="D152" s="5"/>
@@ -2694,7 +2697,7 @@
     <row r="155" ht="24.75" customHeight="1">
       <c r="A155" s="18"/>
       <c r="B155" s="19" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C155" s="29"/>
       <c r="D155" s="5"/>
@@ -2724,7 +2727,7 @@
     <row r="158" ht="24.75" customHeight="1">
       <c r="A158" s="18"/>
       <c r="B158" s="19" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C158" s="29"/>
       <c r="D158" s="5"/>
@@ -2754,7 +2757,7 @@
     <row r="161" ht="24.75" customHeight="1">
       <c r="A161" s="18"/>
       <c r="B161" s="19" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C161" s="29"/>
       <c r="D161" s="5"/>
@@ -2784,7 +2787,7 @@
     <row r="164" ht="24.75" customHeight="1">
       <c r="A164" s="18"/>
       <c r="B164" s="19" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C164" s="29"/>
       <c r="D164" s="5"/>
@@ -2814,7 +2817,7 @@
     <row r="167" ht="24.75" customHeight="1">
       <c r="A167" s="18"/>
       <c r="B167" s="19" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C167" s="29"/>
       <c r="D167" s="5"/>

</xml_diff>

<commit_message>
Fixed documentation bugg(ies) and link in documentation
</commit_message>
<xml_diff>
--- a/inst/googlesheet/emeScheme.xlsx
+++ b/inst/googlesheet/emeScheme.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="143">
   <si>
     <t>Property_Level_1</t>
   </si>
@@ -260,18 +260,27 @@
     <t>ecologicalRoleInTreatment</t>
   </si>
   <si>
+    <t>BacteriaFlagellatesTreatment</t>
+  </si>
+  <si>
     <t>initial density</t>
   </si>
   <si>
     <t>500</t>
   </si>
   <si>
+    <t>TemperatureTreatment</t>
+  </si>
+  <si>
     <t>20-30</t>
   </si>
   <si>
     <t>daily fluctuations</t>
   </si>
   <si>
+    <t>LightTreatment</t>
+  </si>
+  <si>
     <t>colour (nm) [numeric]</t>
   </si>
   <si>
@@ -284,7 +293,7 @@
     <t>change</t>
   </si>
   <si>
-    <t>Nutrients</t>
+    <t>NutrientTreatment</t>
   </si>
   <si>
     <t>changeInTreatment</t>
@@ -1716,7 +1725,7 @@
     <row r="63" ht="24.75" customHeight="1">
       <c r="A63" s="18"/>
       <c r="B63" s="19" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="C63" s="29"/>
       <c r="D63" s="29"/>
@@ -1739,12 +1748,12 @@
       <c r="A65" s="20"/>
       <c r="B65" s="21"/>
       <c r="C65" s="11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D65" s="11"/>
       <c r="E65" s="11"/>
       <c r="F65" s="51" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="66" ht="24.75" customHeight="1">
@@ -1763,7 +1772,7 @@
     <row r="67" ht="24.75" customHeight="1">
       <c r="A67" s="29"/>
       <c r="B67" s="19" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="C67" s="29"/>
       <c r="D67" s="5"/>
@@ -1791,7 +1800,7 @@
       <c r="D69" s="31"/>
       <c r="E69" s="31"/>
       <c r="F69" s="51" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" ht="24.75" customHeight="1">
@@ -1803,13 +1812,13 @@
       <c r="D70" s="31"/>
       <c r="E70" s="31"/>
       <c r="F70" s="51" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="71" ht="24.75" customHeight="1">
       <c r="A71" s="29"/>
       <c r="B71" s="19" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="C71" s="29"/>
       <c r="D71" s="5"/>
@@ -1832,7 +1841,7 @@
       <c r="A73" s="21"/>
       <c r="B73" s="21"/>
       <c r="C73" s="11" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D73" s="31"/>
       <c r="E73" s="31"/>
@@ -1855,7 +1864,7 @@
     <row r="75" ht="24.75" customHeight="1">
       <c r="A75" s="29"/>
       <c r="B75" s="19" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C75" s="29"/>
       <c r="D75" s="5"/>
@@ -1866,7 +1875,7 @@
       <c r="A76" s="21"/>
       <c r="B76" s="21"/>
       <c r="C76" s="11" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D76" s="31"/>
       <c r="E76" s="31"/>
@@ -1876,7 +1885,7 @@
       <c r="A77" s="21"/>
       <c r="B77" s="21"/>
       <c r="C77" s="30" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D77" s="31"/>
       <c r="E77" s="31"/>
@@ -1885,7 +1894,7 @@
     <row r="78" ht="24.75" customHeight="1">
       <c r="A78" s="29"/>
       <c r="B78" s="19" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C78" s="37"/>
       <c r="D78" s="5"/>
@@ -1896,7 +1905,7 @@
       <c r="A79" s="21"/>
       <c r="B79" s="21"/>
       <c r="C79" s="11" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D79" s="31"/>
       <c r="E79" s="31"/>
@@ -1915,7 +1924,7 @@
     <row r="81" ht="24.75" customHeight="1">
       <c r="A81" s="29"/>
       <c r="B81" s="19" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C81" s="38"/>
       <c r="D81" s="5"/>
@@ -1945,7 +1954,7 @@
     <row r="84" ht="24.75" customHeight="1">
       <c r="A84" s="39"/>
       <c r="B84" s="19" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
@@ -1966,7 +1975,7 @@
       <c r="A86" s="32"/>
       <c r="B86" s="28"/>
       <c r="C86" s="35" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D86" s="31"/>
       <c r="E86" s="31"/>
@@ -1976,7 +1985,7 @@
       <c r="A87" s="32"/>
       <c r="B87" s="28"/>
       <c r="C87" s="35" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D87" s="31"/>
       <c r="E87" s="31"/>
@@ -1985,7 +1994,7 @@
     <row r="88" ht="24.75" customHeight="1">
       <c r="A88" s="29"/>
       <c r="B88" s="40" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C88" s="29"/>
       <c r="D88" s="5"/>
@@ -2014,7 +2023,7 @@
     </row>
     <row r="91" ht="24.75" customHeight="1">
       <c r="A91" s="4" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B91" s="29"/>
       <c r="C91" s="29"/>
@@ -2025,7 +2034,7 @@
     <row r="92" ht="24.75" customHeight="1">
       <c r="A92" s="20"/>
       <c r="B92" s="11" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C92" s="21"/>
       <c r="D92" s="31"/>
@@ -2049,18 +2058,18 @@
     <row r="94" ht="24.75" customHeight="1">
       <c r="A94" s="20"/>
       <c r="B94" s="11" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C94" s="21"/>
       <c r="D94" s="31"/>
       <c r="E94" s="31"/>
       <c r="F94" s="51" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="95" ht="24.75" customHeight="1">
       <c r="A95" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B95" s="29"/>
       <c r="C95" s="29"/>
@@ -2071,7 +2080,7 @@
     <row r="96" ht="24.75" customHeight="1">
       <c r="A96" s="18"/>
       <c r="B96" s="19" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C96" s="29"/>
       <c r="D96" s="5"/>
@@ -2087,61 +2096,61 @@
       <c r="D97" s="22"/>
       <c r="E97" s="22"/>
       <c r="F97" s="51" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="98" ht="24.75" customHeight="1">
       <c r="A98" s="20"/>
       <c r="B98" s="21"/>
       <c r="C98" s="11" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D98" s="31"/>
       <c r="E98" s="31"/>
       <c r="F98" s="51" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="99" ht="24.75" customHeight="1">
       <c r="A99" s="20"/>
       <c r="B99" s="21"/>
       <c r="C99" s="11" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D99" s="31"/>
       <c r="E99" s="31"/>
       <c r="F99" s="51" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="100" ht="24.75" customHeight="1">
       <c r="A100" s="20"/>
       <c r="B100" s="21"/>
       <c r="C100" s="11" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D100" s="31"/>
       <c r="E100" s="31"/>
       <c r="F100" s="51" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="101" ht="24.75" customHeight="1">
       <c r="A101" s="20"/>
       <c r="B101" s="21"/>
       <c r="C101" s="35" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D101" s="31"/>
       <c r="E101" s="31"/>
       <c r="F101" s="51" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="102" ht="24.75" customHeight="1">
       <c r="A102" s="18"/>
       <c r="B102" s="19" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C102" s="29"/>
       <c r="D102" s="5"/>
@@ -2164,7 +2173,7 @@
       <c r="A104" s="20"/>
       <c r="B104" s="21"/>
       <c r="C104" s="21" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D104" s="21"/>
       <c r="E104" s="21"/>
@@ -2174,19 +2183,19 @@
       <c r="A105" s="20"/>
       <c r="B105" s="21"/>
       <c r="C105" s="28" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D105" s="21"/>
       <c r="E105" s="21"/>
       <c r="F105" s="51" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="106" ht="24.75" customHeight="1">
       <c r="A106" s="20"/>
       <c r="B106" s="21"/>
       <c r="C106" s="28" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D106" s="21"/>
       <c r="E106" s="21"/>
@@ -2198,19 +2207,19 @@
       <c r="A107" s="20"/>
       <c r="B107" s="21"/>
       <c r="C107" s="28" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D107" s="21"/>
       <c r="E107" s="21"/>
       <c r="F107" s="51" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="108" ht="24.75" customHeight="1">
       <c r="A108" s="20"/>
       <c r="B108" s="21"/>
       <c r="C108" s="28" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D108" s="21"/>
       <c r="E108" s="21"/>
@@ -2220,7 +2229,7 @@
       <c r="A109" s="20"/>
       <c r="B109" s="21"/>
       <c r="C109" s="28" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D109" s="21"/>
       <c r="E109" s="21"/>
@@ -2232,19 +2241,19 @@
       <c r="A110" s="20"/>
       <c r="B110" s="21"/>
       <c r="C110" s="35" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D110" s="21"/>
       <c r="E110" s="21"/>
       <c r="F110" s="51" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="111" ht="24.75" customHeight="1">
       <c r="A111" s="20"/>
       <c r="B111" s="21"/>
       <c r="C111" s="28" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D111" s="21"/>
       <c r="E111" s="21"/>
@@ -2256,7 +2265,7 @@
       <c r="A112" s="20"/>
       <c r="B112" s="21"/>
       <c r="C112" s="35" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D112" s="35"/>
       <c r="E112" s="21"/>
@@ -2268,7 +2277,7 @@
       <c r="A113" s="20"/>
       <c r="B113" s="21"/>
       <c r="C113" s="35" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D113" s="21"/>
       <c r="E113" s="21"/>
@@ -2280,7 +2289,7 @@
       <c r="A114" s="20"/>
       <c r="B114" s="21"/>
       <c r="C114" s="35" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D114" s="21"/>
       <c r="E114" s="21"/>
@@ -2290,19 +2299,19 @@
       <c r="A115" s="20"/>
       <c r="B115" s="21"/>
       <c r="C115" s="35" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D115" s="21"/>
       <c r="E115" s="21"/>
       <c r="F115" s="51" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="116" ht="24.75" customHeight="1">
       <c r="A116" s="20"/>
       <c r="B116" s="21"/>
       <c r="C116" s="35" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D116" s="21"/>
       <c r="E116" s="21"/>
@@ -2311,7 +2320,7 @@
     <row r="117" ht="24.75" customHeight="1">
       <c r="A117" s="18"/>
       <c r="B117" s="40" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C117" s="5"/>
       <c r="D117" s="29"/>
@@ -2332,7 +2341,7 @@
       <c r="A119" s="20"/>
       <c r="B119" s="21"/>
       <c r="C119" s="22" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D119" s="21"/>
       <c r="E119" s="21"/>
@@ -2352,7 +2361,7 @@
       <c r="A121" s="20"/>
       <c r="B121" s="21"/>
       <c r="C121" s="23" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D121" s="21"/>
       <c r="E121" s="21"/>
@@ -2361,7 +2370,7 @@
     <row r="122" ht="24.75" customHeight="1">
       <c r="A122" s="18"/>
       <c r="B122" s="19" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C122" s="29"/>
       <c r="D122" s="5"/>
@@ -2372,7 +2381,7 @@
       <c r="A123" s="20"/>
       <c r="B123" s="41"/>
       <c r="C123" s="11" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D123" s="31"/>
       <c r="E123" s="31"/>
@@ -2392,7 +2401,7 @@
       <c r="A125" s="20"/>
       <c r="B125" s="41"/>
       <c r="C125" s="42" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D125" s="31"/>
       <c r="E125" s="31"/>
@@ -2402,7 +2411,7 @@
       <c r="A126" s="20"/>
       <c r="B126" s="41"/>
       <c r="C126" s="30" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D126" s="31"/>
       <c r="E126" s="31"/>
@@ -2411,7 +2420,7 @@
     <row r="127" ht="24.75" customHeight="1">
       <c r="A127" s="18"/>
       <c r="B127" s="19" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C127" s="29"/>
       <c r="D127" s="5"/>
@@ -2441,7 +2450,7 @@
     <row r="130" ht="24.75" customHeight="1">
       <c r="A130" s="18"/>
       <c r="B130" s="40" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C130" s="29"/>
       <c r="D130" s="5"/>
@@ -2462,7 +2471,7 @@
       <c r="A132" s="20"/>
       <c r="B132" s="44"/>
       <c r="C132" s="11" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D132" s="31"/>
       <c r="E132" s="31"/>
@@ -2471,7 +2480,7 @@
     <row r="133" ht="24.75" customHeight="1">
       <c r="A133" s="18"/>
       <c r="B133" s="19" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C133" s="29"/>
       <c r="D133" s="5"/>
@@ -2482,7 +2491,7 @@
       <c r="A134" s="20"/>
       <c r="B134" s="44"/>
       <c r="C134" s="11" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D134" s="31"/>
       <c r="E134" s="31"/>
@@ -2500,7 +2509,7 @@
     </row>
     <row r="136" ht="24.75" customHeight="1">
       <c r="A136" s="4" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B136" s="29"/>
       <c r="C136" s="29"/>
@@ -2511,7 +2520,7 @@
     <row r="137" ht="24.75" customHeight="1">
       <c r="A137" s="18"/>
       <c r="B137" s="19" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C137" s="29"/>
       <c r="D137" s="5"/>
@@ -2527,7 +2536,7 @@
       <c r="D138" s="31"/>
       <c r="E138" s="31"/>
       <c r="F138" s="51" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="139" ht="24.75" customHeight="1">
@@ -2543,7 +2552,7 @@
     <row r="140" ht="24.75" customHeight="1">
       <c r="A140" s="18"/>
       <c r="B140" s="19" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C140" s="29"/>
       <c r="D140" s="5"/>
@@ -2554,30 +2563,30 @@
       <c r="A141" s="20"/>
       <c r="B141" s="21"/>
       <c r="C141" s="11" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D141" s="11"/>
       <c r="E141" s="11"/>
       <c r="F141" s="51" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="142" ht="24.75" customHeight="1">
       <c r="A142" s="20"/>
       <c r="B142" s="21"/>
       <c r="C142" s="11" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D142" s="11"/>
       <c r="E142" s="11"/>
       <c r="F142" s="51" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="143" ht="24.75" customHeight="1">
       <c r="A143" s="18"/>
       <c r="B143" s="19" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C143" s="5"/>
       <c r="D143" s="5"/>
@@ -2607,7 +2616,7 @@
     <row r="146" ht="24.75" customHeight="1">
       <c r="A146" s="18"/>
       <c r="B146" s="19" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C146" s="29"/>
       <c r="D146" s="5"/>
@@ -2637,7 +2646,7 @@
     <row r="149" ht="24.75" customHeight="1">
       <c r="A149" s="18"/>
       <c r="B149" s="19" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C149" s="29"/>
       <c r="D149" s="5"/>
@@ -2667,7 +2676,7 @@
     <row r="152" ht="24.75" customHeight="1">
       <c r="A152" s="18"/>
       <c r="B152" s="19" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C152" s="29"/>
       <c r="D152" s="5"/>
@@ -2697,7 +2706,7 @@
     <row r="155" ht="24.75" customHeight="1">
       <c r="A155" s="18"/>
       <c r="B155" s="19" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C155" s="29"/>
       <c r="D155" s="5"/>
@@ -2727,7 +2736,7 @@
     <row r="158" ht="24.75" customHeight="1">
       <c r="A158" s="18"/>
       <c r="B158" s="19" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C158" s="29"/>
       <c r="D158" s="5"/>
@@ -2757,7 +2766,7 @@
     <row r="161" ht="24.75" customHeight="1">
       <c r="A161" s="18"/>
       <c r="B161" s="19" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C161" s="29"/>
       <c r="D161" s="5"/>
@@ -2787,7 +2796,7 @@
     <row r="164" ht="24.75" customHeight="1">
       <c r="A164" s="18"/>
       <c r="B164" s="19" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C164" s="29"/>
       <c r="D164" s="5"/>
@@ -2817,7 +2826,7 @@
     <row r="167" ht="24.75" customHeight="1">
       <c r="A167" s="18"/>
       <c r="B167" s="19" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C167" s="29"/>
       <c r="D167" s="5"/>

</xml_diff>